<commit_message>
#carpetas por estudiantes y coordinadores #carpetas por cultivos
</commit_message>
<xml_diff>
--- a/Proyecto_Documentation/cultivos_anual_tabla.xlsx
+++ b/Proyecto_Documentation/cultivos_anual_tabla.xlsx
@@ -182,12 +182,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>ayield</t>
-  </si>
-  <si>
-    <t>applot</t>
-  </si>
-  <si>
     <t>production</t>
   </si>
   <si>
@@ -219,6 +213,12 @@
   </si>
   <si>
     <t>Tabla</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>pricePlot</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -342,6 +348,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +688,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E1" s="5">
         <v>2005</v>
@@ -725,7 +732,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -769,7 +776,7 @@
         <v>45</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
@@ -807,13 +814,13 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -857,7 +864,7 @@
         <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -989,7 +996,7 @@
         <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -1033,7 +1040,7 @@
         <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -1074,10 +1081,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -1118,10 +1125,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1162,10 +1169,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1225,7 +1232,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1258,7 @@
         <v>29</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1262,7 +1269,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>30</v>
@@ -1279,7 +1286,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>30</v>
@@ -1296,7 +1303,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -1312,8 +1319,8 @@
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
+      <c r="C5" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
@@ -1329,8 +1336,8 @@
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
+      <c r="C6" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>33</v>
@@ -1349,7 +1356,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,20 +1381,20 @@
       <c r="C1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>54</v>
+      <c r="G1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>